<commit_message>
modified. Should be ok but p53 is strange
</commit_message>
<xml_diff>
--- a/gbm_Scripts_bmra_u251mg/00_outputs_2020_U251MG/ALL_DATA_2020_Jing_u251mg.xlsx
+++ b/gbm_Scripts_bmra_u251mg/00_outputs_2020_U251MG/ALL_DATA_2020_Jing_u251mg.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="modules" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,210 +28,210 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3078" uniqueCount="1076">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3075" uniqueCount="1076">
   <si>
     <t xml:space="preserve">Module</t>
   </si>
   <si>
+    <t xml:space="preserve">CDK2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CDK4_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EGFR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aurora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estrogen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PDGFR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hypoxia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PI3K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC50, uM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Removed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">roscovitine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dasatinib(not recorded)	PDGFR	1,362	GI1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">palbociclib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alvocidib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LY-294002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AS-605240</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NVP-BEZ235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GDC-0349</t>
+  </si>
+  <si>
+    <t xml:space="preserve">taselisib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PI-103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30nm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AZ-628</t>
+  </si>
+  <si>
+    <t xml:space="preserve">martin's</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD-0325901</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dabrafenib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trametinib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.92 1.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selumetinib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avg 214nm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vandetanib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">500 nm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vemurafenib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRAF 31, CRAF 48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAY-87-2243</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,7nm </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dienestrol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not recorded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAY-10585</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.4 μM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estradiol-cypionate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ponatinib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1 nm multiple targets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">raloxifene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.7 nM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HLI-373</t>
+  </si>
+  <si>
+    <t xml:space="preserve">erlotinib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2nM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAR405838</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.88 ki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gefitinib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">57nm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">serdemetan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">afatinib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10nM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JNJ-7706621</t>
+  </si>
+  <si>
     <t xml:space="preserve">CDK1</t>
   </si>
   <si>
-    <t xml:space="preserve">CDK2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CDK4_6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">p53</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EGFR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aurora</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estrogen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PDGFR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hypoxia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PI3K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drug</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC50, uM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Removed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JNJ-7706621</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dasatinib(not recorded)	PDGFR	1,362	GI1</t>
+    <t xml:space="preserve">entinostat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.51, 1.7 um</t>
   </si>
   <si>
     <t xml:space="preserve">PHA-793887</t>
   </si>
   <si>
-    <t xml:space="preserve">alvocidib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">roscovitine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AS-605240</t>
-  </si>
-  <si>
-    <t xml:space="preserve">palbociclib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GDC-0349</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LY-294002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PI-103</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30nm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NVP-BEZ235</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PD-0325901</t>
-  </si>
-  <si>
-    <t xml:space="preserve">martin's</t>
-  </si>
-  <si>
-    <t xml:space="preserve">taselisib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">trametinib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.92 1.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AZ-628</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vandetanib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">500 nm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dabrafenib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BAY-87-2243</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,7nm </t>
-  </si>
-  <si>
-    <t xml:space="preserve">selumetinib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">avg 214nm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAY-10585</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.4 μM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vemurafenib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BRAF 31, CRAF 48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ponatinib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.1 nm multiple targets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dienestrol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">not recorded</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HLI-373</t>
-  </si>
-  <si>
-    <t xml:space="preserve">estradiol-cypionate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAR405838</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.88 ki</t>
-  </si>
-  <si>
-    <t xml:space="preserve">raloxifene</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.7 nM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serdemetan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">erlotinib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2nM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gefitinib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">57nm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">afatinib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10nM</t>
+    <t xml:space="preserve">panobinostat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5nm</t>
   </si>
   <si>
     <t xml:space="preserve">lapatinib</t>
   </si>
   <si>
     <t xml:space="preserve">	10.8 nM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">entinostat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.51, 1.7 um</t>
-  </si>
-  <si>
-    <t xml:space="preserve">panobinostat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5nm</t>
   </si>
   <si>
     <t xml:space="preserve">vorinostat</t>
@@ -3317,17 +3317,17 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
+      <b val="true"/>
       <sz val="11"/>
-      <color rgb="FF0563C1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <u val="single"/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color rgb="FF0563C1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -3417,7 +3417,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -3454,19 +3454,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3482,19 +3482,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3502,7 +3502,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3616,13 +3616,13 @@
   </sheetPr>
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.65"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3638,13 +3638,13 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="4"/>
@@ -3665,7 +3665,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="0" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3675,7 +3675,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -3684,11 +3684,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
@@ -3714,10 +3710,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+      <selection pane="bottomLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9"/>
@@ -3727,189 +3723,190 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="5" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7" t="n">
-        <v>0.027</v>
-      </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="10"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="7"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="10" t="n">
+        <v>0.045</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7" t="n">
-        <v>0.18</v>
-      </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="9" t="s">
+      <c r="F3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="10" t="n">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="8" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="8" t="n">
+        <v>0.1595</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="8" t="n">
+        <v>1.71</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="G3" s="7" t="n">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="10" t="n">
-        <v>0.1595</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="7" t="n">
-        <v>0.045</v>
-      </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="0" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="10" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="11" t="n">
+        <v>0.00262</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="10" t="n">
-        <v>1.36</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>25</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>0.09</v>
       </c>
       <c r="H6" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="10" t="n">
-        <v>1.71</v>
-      </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="7" t="s">
         <v>28</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G7" s="11" t="n">
         <v>0.015</v>
       </c>
       <c r="H7" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="8" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="11" t="n">
-        <v>0.00262</v>
-      </c>
-      <c r="E8" s="9" t="s">
+      <c r="F8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="8" t="n">
+        <v>0.00408</v>
+      </c>
+      <c r="H8" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="10" t="n">
-        <v>0.00408</v>
-      </c>
-      <c r="H8" s="0" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="s">
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="8" t="n">
+        <v>0.643</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>34</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G9" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="G9" s="8" t="n">
         <v>1.5</v>
       </c>
       <c r="H9" s="0" t="s">
@@ -3917,74 +3914,77 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="10" t="n">
-        <v>0.1</v>
+        <v>9</v>
+      </c>
+      <c r="C10" s="8" t="n">
+        <v>0.1185</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>37</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G10" s="11" t="n">
         <v>0.0021</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="s">
-        <v>39</v>
+      <c r="A11" s="7" t="s">
+        <v>40</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="10" t="n">
-        <v>0.643</v>
+        <v>6</v>
+      </c>
+      <c r="C11" s="11" t="n">
+        <v>200</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G11" s="13" t="n">
         <v>13.2</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="s">
-        <v>43</v>
+      <c r="A12" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="10" t="n">
-        <v>0.1185</v>
+        <v>6</v>
+      </c>
+      <c r="C12" s="11" t="n">
+        <v>200</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>45</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="10" t="n">
+        <v>7</v>
+      </c>
+      <c r="G12" s="8" t="n">
         <v>0.0033</v>
       </c>
       <c r="H12" s="0" t="s">
@@ -3992,307 +3992,289 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="7" t="s">
         <v>47</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="11" t="n">
-        <v>200</v>
+        <v>6</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0.0171</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="9" t="s">
         <v>49</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G13" s="11" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="11" t="n">
-        <v>200</v>
+        <v>4</v>
+      </c>
+      <c r="C14" s="10" t="n">
+        <v>0.006</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="8" t="s">
         <v>51</v>
       </c>
+      <c r="E14" s="9" t="s">
+        <v>52</v>
+      </c>
       <c r="F14" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G14" s="11" t="n">
         <v>0.0264</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9" t="s">
-        <v>53</v>
+      <c r="A15" s="12" t="s">
+        <v>54</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="0" t="n">
-        <v>0.0171</v>
+        <v>4</v>
+      </c>
+      <c r="C15" s="8" t="n">
+        <v>0.171</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G15" s="0" t="n">
         <v>62.15</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9" t="s">
-        <v>56</v>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="10" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" s="10" t="n">
+        <v>0.027</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>3.315</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" s="10" t="n">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="8" t="n">
+        <v>0.0324</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+    </row>
+    <row r="20" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="16" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+    </row>
+    <row r="21" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="16" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+    </row>
+    <row r="22" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>2.13</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="7" t="n">
-        <v>0.006</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-    </row>
-    <row r="17" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B17" s="1" t="s">
+      <c r="C23" s="11" t="n">
+        <v>0.00111</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="10" t="n">
-        <v>0.171</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-    </row>
-    <row r="18" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="7" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-    </row>
-    <row r="19" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="10" t="n">
-        <v>0.0324</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-    </row>
-    <row r="20" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="0" t="n">
-        <v>3.315</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-    </row>
-    <row r="21" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="0" t="n">
-        <v>0.015</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-    </row>
-    <row r="22" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="0" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="16" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="16" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>73</v>
+      <c r="C24" s="17" t="n">
+        <v>0.0232</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>8</v>
+      <c r="A25" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>2.13</v>
+        <v>0.0018</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="9" t="s">
-        <v>76</v>
+      <c r="A26" s="7" t="s">
+        <v>82</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C26" s="11" t="n">
-        <v>0.00111</v>
+        <v>0.54</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="9" t="s">
-        <v>78</v>
+      <c r="A27" s="7" t="s">
+        <v>84</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="17" t="n">
-        <v>0.0232</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="0" t="n">
-        <v>0.0018</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="11" t="n">
-        <v>0.54</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="C27" s="8" t="n">
         <v>9.75</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D27" s="0" t="s">
         <v>85</v>
       </c>
     </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4308,29 +4290,29 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="5"/>
-      <c r="C42" s="10"/>
+      <c r="C42" s="8"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="5"/>
-      <c r="C44" s="10"/>
+      <c r="C44" s="8"/>
     </row>
     <row r="47" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C47" s="14"/>
+      <c r="C47" s="15"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1" display="AS-605240"/>
-    <hyperlink ref="E5" r:id="rId2" display="GDC-0349"/>
-    <hyperlink ref="A6" r:id="rId3" display="LY-294002"/>
-    <hyperlink ref="A7" r:id="rId4" display="NVP-BEZ235"/>
-    <hyperlink ref="A8" r:id="rId5" display="taselisib"/>
+    <hyperlink ref="A4" r:id="rId1" display="LY-294002"/>
+    <hyperlink ref="E4" r:id="rId2" display="AS-605240"/>
+    <hyperlink ref="A5" r:id="rId3" display="NVP-BEZ235"/>
+    <hyperlink ref="E5" r:id="rId4" display="GDC-0349"/>
+    <hyperlink ref="A6" r:id="rId5" display="taselisib"/>
     <hyperlink ref="E9" r:id="rId6" display="vandetanib"/>
     <hyperlink ref="E13" r:id="rId7" display="HLI-373"/>
     <hyperlink ref="E14" r:id="rId8" display="SAR405838"/>
-    <hyperlink ref="A17" r:id="rId9" display="gefitinib"/>
-    <hyperlink ref="A18" r:id="rId10" display="afatinib"/>
-    <hyperlink ref="A19" r:id="rId11" display="lapatinib"/>
-    <hyperlink ref="A28" r:id="rId12" display="AMG-232"/>
+    <hyperlink ref="A15" r:id="rId9" display="gefitinib"/>
+    <hyperlink ref="A16" r:id="rId10" display="afatinib"/>
+    <hyperlink ref="E18" r:id="rId11" display="lapatinib"/>
+    <hyperlink ref="A25" r:id="rId12" display="AMG-232"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -4355,14 +4337,14 @@
       <selection pane="bottomLeft" activeCell="K823" activeCellId="0" sqref="K823"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="13.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="18" width="26"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
+    <row r="1" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
         <v>86</v>
       </c>
       <c r="B1" s="19" t="s">
@@ -7503,7 +7485,7 @@
         <v>0.0274486987980314</v>
       </c>
       <c r="G137" s="20" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="H137" s="0" t="n">
         <v>0</v>
@@ -7549,7 +7531,7 @@
         <v>0.0273629915153805</v>
       </c>
       <c r="G139" s="20" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H139" s="0" t="n">
         <v>0.0548317671833257</v>
@@ -8020,7 +8002,7 @@
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="B160" s="18" t="n">
         <v>0.00839205108451629</v>
@@ -10470,7 +10452,7 @@
         <v>0.014334137570997</v>
       </c>
       <c r="G266" s="20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H266" s="0" t="n">
         <v>-0.0282494708004371</v>
@@ -14759,7 +14741,7 @@
     </row>
     <row r="453" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="0" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B453" s="18" t="n">
         <v>-0.0105417720464063</v>
@@ -20486,7 +20468,7 @@
     </row>
     <row r="702" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A702" s="0" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B702" s="18" t="n">
         <v>0.0270529462064025</v>
@@ -26555,7 +26537,7 @@
       <selection pane="topLeft" activeCell="M30" activeCellId="0" sqref="M30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="8.67"/>
   </cols>
@@ -27332,7 +27314,7 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="21" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>0</v>
@@ -27398,7 +27380,7 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="21" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B77" s="0" t="n">
         <v>0.0548317671833257</v>
@@ -28014,7 +27996,7 @@
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B133" s="0" t="n">
         <v>-0.0282494708004371</v>
@@ -37351,25 +37333,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
@@ -37381,25 +37364,22 @@
       <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
-        <v>11</v>
+      <c r="L1" s="4" t="s">
+        <v>1067</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>1067</v>
-      </c>
-      <c r="N1" s="4" t="s">
         <v>1068</v>
       </c>
     </row>
@@ -37443,12 +37423,9 @@
       <c r="M2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="N2" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -37487,12 +37464,9 @@
       <c r="M3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="N3" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="0" t="n">
@@ -37529,9 +37503,6 @@
         <v>0</v>
       </c>
       <c r="M4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -37575,9 +37546,6 @@
       <c r="M5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="N5" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
@@ -37619,9 +37587,6 @@
       <c r="M6" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="N6" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
@@ -37663,12 +37628,9 @@
       <c r="M7" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="N7" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="0" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="0" t="n">
@@ -37705,9 +37667,6 @@
         <v>0</v>
       </c>
       <c r="M8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N8" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -37751,12 +37710,9 @@
       <c r="M9" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="N9" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="0" t="n">
@@ -37793,9 +37749,6 @@
         <v>0</v>
       </c>
       <c r="M10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N10" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -37839,13 +37792,10 @@
       <c r="M11" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="N11" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
-        <v>11</v>
+      <c r="A12" s="4" t="s">
+        <v>1067</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0</v>
@@ -37881,15 +37831,12 @@
         <v>0</v>
       </c>
       <c r="M12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N12" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0</v>
@@ -37927,54 +37874,8 @@
       <c r="M13" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="N13" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
-        <v>1068</v>
-      </c>
-      <c r="B14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N14" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -37997,20 +37898,20 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.65"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>1069</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>1070</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>1071</v>
       </c>
     </row>
@@ -38041,7 +37942,7 @@
         <v>1075</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>3.33</v>

</xml_diff>

<commit_message>
updates u251mg removed hypoxia
</commit_message>
<xml_diff>
--- a/gbm_Scripts_bmra_u251mg/00_outputs_2020_U251MG/ALL_DATA_2020_Jing_u251mg.xlsx
+++ b/gbm_Scripts_bmra_u251mg/00_outputs_2020_U251MG/ALL_DATA_2020_Jing_u251mg.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3075" uniqueCount="1077">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3073" uniqueCount="1077">
   <si>
     <t xml:space="preserve">Module</t>
   </si>
@@ -3623,7 +3623,7 @@
       <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.65"/>
   </cols>
@@ -3713,10 +3713,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M11" activeCellId="0" sqref="M11"/>
+      <selection pane="bottomLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9"/>
@@ -4328,7 +4328,7 @@
       <selection pane="bottomLeft" activeCell="K823" activeCellId="0" sqref="K823"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="13.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="18" width="26"/>
@@ -26528,7 +26528,7 @@
       <selection pane="topLeft" activeCell="M30" activeCellId="0" sqref="M30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="8.67"/>
   </cols>
@@ -37324,16 +37324,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M1048576"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37358,19 +37358,16 @@
       <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
-        <v>8</v>
+      <c r="I1" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="K1" s="4" t="s">
+        <v>1068</v>
+      </c>
       <c r="L1" s="4" t="s">
-        <v>1068</v>
-      </c>
-      <c r="M1" s="4" t="s">
         <v>1069</v>
       </c>
     </row>
@@ -37411,9 +37408,6 @@
       <c r="L2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M2" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -37452,9 +37446,6 @@
       <c r="L3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M3" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
@@ -37493,9 +37484,6 @@
       <c r="L4" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M4" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
@@ -37534,9 +37522,6 @@
       <c r="L5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M5" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
@@ -37575,9 +37560,6 @@
       <c r="L6" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M6" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
@@ -37616,9 +37598,6 @@
       <c r="L7" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M7" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -37657,13 +37636,10 @@
       <c r="L8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M8" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>8</v>
+      <c r="A9" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0</v>
@@ -37696,15 +37672,12 @@
         <v>0</v>
       </c>
       <c r="L9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0</v>
@@ -37739,13 +37712,10 @@
       <c r="L10" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M10" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
-        <v>10</v>
+      <c r="A11" s="4" t="s">
+        <v>1068</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0</v>
@@ -37778,15 +37748,12 @@
         <v>0</v>
       </c>
       <c r="L11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M11" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0</v>
@@ -37821,52 +37788,7 @@
       <c r="L12" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M12" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
-        <v>1069</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M13" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -37889,7 +37811,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.64"/>

</xml_diff>

<commit_message>
Removed now p53 and parp, still got EGFR and Aurora strange ummmmm
</commit_message>
<xml_diff>
--- a/gbm_Scripts_bmra_u251mg/00_outputs_2020_U251MG/ALL_DATA_2020_Jing_u251mg.xlsx
+++ b/gbm_Scripts_bmra_u251mg/00_outputs_2020_U251MG/ALL_DATA_2020_Jing_u251mg.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="modules" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3085" uniqueCount="1082">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3079" uniqueCount="1082">
   <si>
     <t xml:space="preserve">Module</t>
   </si>
@@ -39,271 +39,271 @@
     <t xml:space="preserve">CDK4_6</t>
   </si>
   <si>
+    <t xml:space="preserve">EGFR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aurora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estrogen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PDGFR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hypoxia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PI3K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC50, uM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Removed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">roscovitine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dasatinib(not recorded)	PDGFR	1,362	GI1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">palbociclib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alvocidib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LY-294002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AS-605240</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NVP-BEZ235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GDC-0349</t>
+  </si>
+  <si>
+    <t xml:space="preserve">taselisib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PI-103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30nm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AZ-628</t>
+  </si>
+  <si>
+    <t xml:space="preserve">martin's</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD-0325901</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dabrafenib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trametinib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.92 1.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vemurafenib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRAF 31, CRAF 48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vandetanib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">500 nm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dienestrol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not recorded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAY-87-2243</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,7nm </t>
+  </si>
+  <si>
+    <t xml:space="preserve">estradiol-cypionate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAY-10585</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.4 μM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">erlotinib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2nM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ponatinib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1 nm multiple targets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gefitinib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">57nm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HLI-373</t>
+  </si>
+  <si>
     <t xml:space="preserve">p53</t>
   </si>
   <si>
-    <t xml:space="preserve">EGFR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aurora</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estrogen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PDGFR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hypoxia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PI3K</t>
+    <t xml:space="preserve">imatinib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100nm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAR405838</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.88 ki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tandutinib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.20 μM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">serdemetan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">masitinib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avg 710nm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JNJ-7706621</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CDK1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">barasertib-HQPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.37nm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHA-793887</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tozasertib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avg 7,73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lapatinib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	10.8 nM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">entinostat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.51, 1.7 um</t>
+  </si>
+  <si>
+    <t xml:space="preserve">panobinostat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5nm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vorinostat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10nm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selumetinib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avg 214nm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">afatinib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10nM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RITA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">viability(colon,prostate cancer)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">raloxifene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.7 nM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMG-232</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.6 nM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nutlin-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">180nm cell free</t>
+  </si>
+  <si>
+    <t xml:space="preserve">olaparib</t>
   </si>
   <si>
     <t xml:space="preserve">PARP</t>
   </si>
   <si>
-    <t xml:space="preserve">Drug</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC50, uM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Removed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">roscovitine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dasatinib(not recorded)	PDGFR	1,362	GI1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">palbociclib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">alvocidib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LY-294002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AS-605240</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NVP-BEZ235</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GDC-0349</t>
-  </si>
-  <si>
-    <t xml:space="preserve">taselisib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PI-103</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30nm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AZ-628</t>
-  </si>
-  <si>
-    <t xml:space="preserve">martin's</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PD-0325901</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dabrafenib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">trametinib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.92 1.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vemurafenib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BRAF 31, CRAF 48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vandetanib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">500 nm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dienestrol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">not recorded</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BAY-87-2243</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,7nm </t>
-  </si>
-  <si>
-    <t xml:space="preserve">estradiol-cypionate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAY-10585</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.4 μM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">erlotinib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2nM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ponatinib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.1 nm multiple targets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gefitinib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">57nm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HLI-373</t>
-  </si>
-  <si>
-    <t xml:space="preserve">imatinib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100nm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAR405838</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.88 ki</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tandutinib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.20 μM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serdemetan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">masitinib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">avg 710nm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JNJ-7706621</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CDK1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">barasertib-HQPA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.37nm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHA-793887</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tozasertib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">avg 7,73</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lapatinib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	10.8 nM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AMG-232</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.6 nM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">entinostat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HDAC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.51, 1.7 um</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nutlin-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">180nm cell free</t>
-  </si>
-  <si>
-    <t xml:space="preserve">panobinostat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5nm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">olaparib</t>
-  </si>
-  <si>
     <t xml:space="preserve">1nm,5nm</t>
   </si>
   <si>
-    <t xml:space="preserve">vorinostat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10nm</t>
-  </si>
-  <si>
     <t xml:space="preserve">rucaparib</t>
   </si>
   <si>
     <t xml:space="preserve">Pmid 34039959</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selumetinib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">avg 214nm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">afatinib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10nM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RITA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">viability(colon,prostate cancer)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">raloxifene</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.7 nM</t>
   </si>
   <si>
     <t xml:space="preserve">Gene</t>
@@ -3634,11 +3634,11 @@
   </sheetPr>
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.65"/>
   </cols>
@@ -3678,7 +3678,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="0" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3688,7 +3688,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3697,16 +3697,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
@@ -3732,10 +3724,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+      <selection pane="bottomLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9"/>
@@ -3745,24 +3737,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -3772,13 +3764,13 @@
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F2" s="10"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -3788,7 +3780,7 @@
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>2</v>
@@ -3799,19 +3791,19 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="8" t="n">
         <v>1.36</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G4" s="8" t="n">
         <v>0.1595</v>
@@ -3819,19 +3811,19 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="8" t="n">
         <v>1.71</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G5" s="8" t="n">
         <v>3</v>
@@ -3839,198 +3831,198 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="11" t="n">
         <v>0.00262</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>0.09</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="8" t="n">
         <v>3</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G7" s="11" t="n">
         <v>0.015</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="8" t="n">
         <v>0.1</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G8" s="8" t="n">
         <v>0.00408</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="8" t="n">
         <v>0.1185</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G9" s="8" t="n">
         <v>1.5</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" s="11" t="n">
         <v>200</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G10" s="11" t="n">
         <v>0.0021</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="11" t="n">
         <v>200</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G11" s="13" t="n">
         <v>13.2</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12" s="10" t="n">
         <v>0.006</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G12" s="8" t="n">
         <v>0.0033</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13" s="8" t="n">
         <v>0.171</v>
       </c>
       <c r="D13" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>3</v>
       </c>
       <c r="G13" s="11" t="n">
         <v>3</v>
@@ -4038,48 +4030,48 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" s="14" t="n">
         <v>0.3</v>
       </c>
       <c r="D14" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>53</v>
-      </c>
       <c r="F14" s="5" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="G14" s="11" t="n">
         <v>0.0264</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="14" t="n">
         <v>0.6</v>
       </c>
       <c r="D15" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="0" t="s">
-        <v>57</v>
-      </c>
       <c r="F15" s="5" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="G15" s="0" t="n">
         <v>62.15</v>
@@ -4087,22 +4079,22 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>2.13</v>
       </c>
       <c r="D16" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="F16" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>61</v>
       </c>
       <c r="G16" s="10" t="n">
         <v>0.027</v>
@@ -4110,22 +4102,22 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" s="11" t="n">
         <v>0.00111</v>
       </c>
       <c r="D17" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>64</v>
-      </c>
       <c r="F17" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G17" s="10" t="n">
         <v>0.18</v>
@@ -4133,192 +4125,196 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18" s="15" t="n">
         <v>0.0232</v>
       </c>
       <c r="D18" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E18" s="12" t="s">
-        <v>67</v>
-      </c>
       <c r="F18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G18" s="8" t="n">
         <v>0.0324</v>
       </c>
       <c r="H18" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="16" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="12" t="s">
+      <c r="F19" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="0" t="n">
-        <v>0.0018</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>72</v>
       </c>
       <c r="G19" s="0" t="n">
         <v>3.315</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="11" t="n">
-        <v>0.54</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>75</v>
-      </c>
       <c r="E20" s="16" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G20" s="0" t="n">
         <v>0.015</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="0" t="n">
-        <v>0.009</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>79</v>
-      </c>
       <c r="E21" s="16" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G21" s="0" t="n">
         <v>0.03</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>83</v>
-      </c>
       <c r="E22" s="7" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G22" s="8" t="n">
         <v>0.643</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="0" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>26</v>
-      </c>
       <c r="E23" s="12" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G23" s="10" t="n">
         <v>0.03</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E24" s="7" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="G24" s="8" t="n">
         <v>9.75</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E25" s="7" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G25" s="0" t="n">
         <v>0.0171</v>
       </c>
       <c r="H25" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E26" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>0.0018</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E27" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G27" s="11" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E28" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <v>0.009</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E29" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="H29" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4356,8 +4352,8 @@
     <hyperlink ref="E13" r:id="rId8" display="HLI-373"/>
     <hyperlink ref="E14" r:id="rId9" display="SAR405838"/>
     <hyperlink ref="E18" r:id="rId10" display="lapatinib"/>
-    <hyperlink ref="A19" r:id="rId11" display="AMG-232"/>
-    <hyperlink ref="E23" r:id="rId12" display="afatinib"/>
+    <hyperlink ref="E23" r:id="rId11" display="afatinib"/>
+    <hyperlink ref="E26" r:id="rId12" display="AMG-232"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -4382,7 +4378,7 @@
       <selection pane="bottomLeft" activeCell="K823" activeCellId="0" sqref="K823"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="13.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="18" width="26"/>
@@ -7530,7 +7526,7 @@
         <v>0.0274486987980314</v>
       </c>
       <c r="G137" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H137" s="0" t="n">
         <v>0</v>
@@ -8047,7 +8043,7 @@
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B160" s="18" t="n">
         <v>0.00839205108451629</v>
@@ -10497,7 +10493,7 @@
         <v>0.014334137570997</v>
       </c>
       <c r="G266" s="20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H266" s="0" t="n">
         <v>-0.0282494708004371</v>
@@ -20513,7 +20509,7 @@
     </row>
     <row r="702" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A702" s="0" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B702" s="18" t="n">
         <v>0.0270529462064025</v>
@@ -26582,7 +26578,7 @@
       <selection pane="topLeft" activeCell="M30" activeCellId="0" sqref="M30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="8.67"/>
   </cols>
@@ -27359,7 +27355,7 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>0</v>
@@ -28041,7 +28037,7 @@
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B133" s="0" t="n">
         <v>-0.0282494708004371</v>
@@ -37378,13 +37374,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F33" activeCellId="0" sqref="F33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
@@ -37406,25 +37402,19 @@
       <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
-        <v>7</v>
+      <c r="H1" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>1073</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>1074</v>
       </c>
     </row>
@@ -37462,12 +37452,6 @@
       <c r="K2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="L2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -37503,12 +37487,6 @@
       <c r="K3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="L3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
@@ -37544,12 +37522,6 @@
       <c r="K4" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="L4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
@@ -37585,12 +37557,6 @@
       <c r="K5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="L5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
@@ -37626,15 +37592,9 @@
       <c r="K6" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="L6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M6" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="0" t="n">
@@ -37667,16 +37627,10 @@
       <c r="K7" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="L7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>7</v>
+      <c r="A8" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0</v>
@@ -37706,12 +37660,6 @@
         <v>0</v>
       </c>
       <c r="K8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M8" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -37749,16 +37697,10 @@
       <c r="K9" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="L9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
-        <v>10</v>
+      <c r="A10" s="4" t="s">
+        <v>1073</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0</v>
@@ -37790,16 +37732,10 @@
       <c r="K10" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="L10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>11</v>
+      <c r="A11" s="4" t="s">
+        <v>1074</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0</v>
@@ -37829,94 +37765,6 @@
         <v>0</v>
       </c>
       <c r="K11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M11" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
-        <v>1073</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M12" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
-        <v>1074</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M13" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -37942,7 +37790,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.64"/>
@@ -37986,7 +37834,7 @@
         <v>1081</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>3.33</v>

</xml_diff>